<commit_message>
Fixed utils error and sucess mesages
</commit_message>
<xml_diff>
--- a/app/files/cms_bulk.xlsx
+++ b/app/files/cms_bulk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javierjaramillo/Desktop/mech-tech-dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/javierjaramillo/Desktop/mech-tech-dashboard/app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AB88C25-1862-9340-82DF-58A74F2FCA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5EDD74-228A-F84A-BE40-C48866D9B16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms_bulk" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -50,19 +50,10 @@
     <t>Nos estamos cuminicando del departamento de finanzas de Meth-Tech para dejarle saber que tiene un pago a cancelar de 100 usd.</t>
   </si>
   <si>
-    <t>Jazmin</t>
-  </si>
-  <si>
     <t>Nos estamos cuminicando del departamento de finanzas de Meth-Tech para dejarle saber que tiene un pago a cancelar de 50 usd.</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
     <t>Nos estamos cuminicando del departamento de finanzas de Meth-Tech para dejarle saber que tiene un pago a cancelar de 200 usd.</t>
-  </si>
-  <si>
-    <t>Francisco</t>
   </si>
   <si>
     <t>Nos estamos cuminicando del departamento de finanzas de Meth-Tech para dejarle saber que tiene un pago a cancelar de 500 usd.</t>
@@ -77,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -555,8 +546,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -911,15 +903,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -930,7 +927,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
@@ -941,47 +938,38 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
       <c r="B3">
         <v>13472399026</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
       <c r="B4">
         <v>13472399026</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
       <c r="B5">
         <v>13472399026</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
+      <c r="A6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
         <v>13472399026</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>